<commit_message>
ya la 2.2 del informe xd
</commit_message>
<xml_diff>
--- a/TABLAS.xlsx
+++ b/TABLAS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GABOID\Estructura-de-datos-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F813F56A-9764-4FCC-893A-BAE83CE77593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E4230B-5000-4252-B05A-782F751CCE38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="106">
   <si>
     <t>Productos</t>
   </si>
@@ -197,6 +197,162 @@
   </si>
   <si>
     <t>Permiso</t>
+  </si>
+  <si>
+    <t>Identificador único para cada producto.</t>
+  </si>
+  <si>
+    <t>Nombre del producto.</t>
+  </si>
+  <si>
+    <t>Descripción detallada del producto.</t>
+  </si>
+  <si>
+    <t>Cantidad total en el inventario.</t>
+  </si>
+  <si>
+    <t>Precio de costo del producto.</t>
+  </si>
+  <si>
+    <t>Relación con el proveedor del producto.</t>
+  </si>
+  <si>
+    <t>Fecha en que el producto fue registrado.</t>
+  </si>
+  <si>
+    <t>Identificador único para cada categoría.</t>
+  </si>
+  <si>
+    <t>Nombre de la categoría (por ejm, "Lentes de Sol","monturas"…)</t>
+  </si>
+  <si>
+    <t>Descripción de la categoría</t>
+  </si>
+  <si>
+    <t>Relación con la tabla Productos</t>
+  </si>
+  <si>
+    <t>Relación con la tabla Categorías.</t>
+  </si>
+  <si>
+    <t>Identificador único para cada local.</t>
+  </si>
+  <si>
+    <t>Nombre del local</t>
+  </si>
+  <si>
+    <t>Ubicación física del local.</t>
+  </si>
+  <si>
+    <t>Número de contacto del local.</t>
+  </si>
+  <si>
+    <t>Identificador único para el registro en el inventario.</t>
+  </si>
+  <si>
+    <t>Relación con el producto.</t>
+  </si>
+  <si>
+    <t>Relación con el local.</t>
+  </si>
+  <si>
+    <t>Cantidad de este producto en el local específico.</t>
+  </si>
+  <si>
+    <t>Fecha de la última actualización, para tener un seguimiento del inventario por local</t>
+  </si>
+  <si>
+    <t>Identificador único del proveedor.</t>
+  </si>
+  <si>
+    <t>Nombre de la empresa proveedora.</t>
+  </si>
+  <si>
+    <t>Nombre de la persona de contacto en el proveedor.</t>
+  </si>
+  <si>
+    <t>Teléfono del proveedor.</t>
+  </si>
+  <si>
+    <t>Correo electrónico del proveedor.</t>
+  </si>
+  <si>
+    <t>Dirección física del proveedor.</t>
+  </si>
+  <si>
+    <t>Detalles sobre las condiciones de entrega o tiempos de despacho.</t>
+  </si>
+  <si>
+    <t>Identificador único para cada movimiento.</t>
+  </si>
+  <si>
+    <t>Relación con el producto involucrado</t>
+  </si>
+  <si>
+    <t>Relación con el local donde ocurre el movimiento.</t>
+  </si>
+  <si>
+    <t>Tipo de movimiento (“entrada” o “salida”).</t>
+  </si>
+  <si>
+    <t>Cantidad involucrada en el movimiento.</t>
+  </si>
+  <si>
+    <t>Fecha del movimiento</t>
+  </si>
+  <si>
+    <t>Identificador del usuario responsable del movimiento.</t>
+  </si>
+  <si>
+    <t>Observaciones adicionales sobre el movimiento</t>
+  </si>
+  <si>
+    <t>Identificador único para cada usuario.</t>
+  </si>
+  <si>
+    <t>Nombre de usuario para iniciar sesión.</t>
+  </si>
+  <si>
+    <t>Contraseña encriptada para el usuario. Correo</t>
+  </si>
+  <si>
+    <t>Correo del usuario</t>
+  </si>
+  <si>
+    <t>Relación con la tabla Roles para asignar el rol al usuario.</t>
+  </si>
+  <si>
+    <t>Fecha en que se creó el usuario.</t>
+  </si>
+  <si>
+    <t>Imagen o Foto del usuario</t>
+  </si>
+  <si>
+    <t>Identificador único para cada rol.</t>
+  </si>
+  <si>
+    <t>rol (por ejemplo, "Administrador", "Empleado", "Supervisor")</t>
+  </si>
+  <si>
+    <t>Descripción del rol.</t>
+  </si>
+  <si>
+    <t>Identificador único para cada controlador o sección de la aplicación.</t>
+  </si>
+  <si>
+    <t>Nombre del controlador (por ejemplo, "Gestión de Productos", "Reportes", "Usuarios").</t>
+  </si>
+  <si>
+    <t>Descripción de la funcionalidad del controlador.</t>
+  </si>
+  <si>
+    <t>Relación con la tabla Roles.</t>
+  </si>
+  <si>
+    <t>Relación con la tabla Controladores.</t>
+  </si>
+  <si>
+    <t>Valor booleano o de texto (por ejemplo, "Lectura", "Escritura", "Completo") que especifica el nivel de acceso.</t>
   </si>
 </sst>
 </file>
@@ -212,7 +368,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,6 +396,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -339,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -353,12 +521,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -366,13 +528,38 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,525 +840,902 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:G60"/>
+  <dimension ref="C3:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="16.77734375" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" customWidth="1"/>
     <col min="4" max="4" width="18.21875" customWidth="1"/>
-    <col min="6" max="6" width="24.77734375" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" customWidth="1"/>
+    <col min="6" max="6" width="46.88671875" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C4" s="4" t="s">
+      <c r="E3" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="23"/>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C5" s="5" t="s">
+      <c r="D4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="24"/>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C6" s="5" t="s">
+      <c r="D5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="24"/>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C7" s="5" t="s">
+      <c r="D6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="24"/>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C7" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C8" s="5" t="s">
+      <c r="E7" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="24"/>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C8" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C9" s="5" t="s">
+      <c r="E8" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="24"/>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C9" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C10" s="6" t="s">
+      <c r="E9" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="24"/>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C10" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F11" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D10" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="24"/>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="4" t="s">
+      <c r="E12" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="26"/>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C14" s="10" t="s">
+      <c r="E13" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="25"/>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C15" s="5" t="s">
+      <c r="E14" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="25"/>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D15" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="25"/>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C18" s="4" t="s">
+      <c r="E17" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="26"/>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C18" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C19" s="11" t="s">
+      <c r="E18" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="25"/>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="E19" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="25"/>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C20" s="5"/>
       <c r="D20" s="8"/>
-      <c r="F20" s="18" t="s">
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C22" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="26"/>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C23" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="25"/>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C24" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="25"/>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C25" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="25"/>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C26" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="25"/>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C27" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="25"/>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C29" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C30" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C31" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C32" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C33" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C34" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C36" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F36" s="26"/>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C37" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="F37" s="25"/>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C38" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="F38" s="25"/>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C39" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F21" s="18" t="s">
+      <c r="D39" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="F39" s="25"/>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C40" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F22" s="18" t="s">
+      <c r="D40" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="F40" s="25"/>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C41" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="G22" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F23" s="18" t="s">
+      <c r="D41" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="F41" s="25"/>
+    </row>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C42" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="G23" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F24" s="19" t="s">
+      <c r="D42" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="F42" s="25"/>
+    </row>
+    <row r="43" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C43" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="G24" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F26" s="21" t="s">
+      <c r="D43" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="F43" s="25"/>
+    </row>
+    <row r="45" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C45" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G26" s="20" t="s">
+      <c r="D45" s="16" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F27" s="4" t="s">
+      <c r="E45" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F45" s="26"/>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C46" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F28" s="5" t="s">
+      <c r="D46" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="F46" s="25"/>
+    </row>
+    <row r="47" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C47" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="D47" s="12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F29" s="5" t="s">
+      <c r="E47" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F47" s="25"/>
+    </row>
+    <row r="48" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C48" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="D48" s="12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F30" s="5" t="s">
+      <c r="E48" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="F48" s="25"/>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C49" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G30" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F31" s="5" t="s">
+      <c r="D49" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="F49" s="25"/>
+    </row>
+    <row r="50" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C50" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="G31" s="8" t="s">
+      <c r="D50" s="12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F32" s="5" t="s">
+      <c r="E50" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="F50" s="25"/>
+    </row>
+    <row r="51" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C51" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="D51" s="12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F33" s="5" t="s">
+      <c r="E51" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="F51" s="25"/>
+    </row>
+    <row r="52" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C52" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="G33" s="8" t="s">
+      <c r="D52" s="12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F34" s="6" t="s">
+      <c r="E52" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="F52" s="25"/>
+    </row>
+    <row r="53" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C53" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G34" s="24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F36" s="2" t="s">
+      <c r="D53" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F53" s="25"/>
+    </row>
+    <row r="55" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C55" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G36" s="20" t="s">
+      <c r="D55" s="16" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F37" s="17" t="s">
+      <c r="E55" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F55" s="26"/>
+    </row>
+    <row r="56" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C56" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="G37" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F38" s="18" t="s">
+      <c r="D56" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="F56" s="25"/>
+    </row>
+    <row r="57" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C57" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G38" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F39" s="18" t="s">
+      <c r="D57" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="F57" s="25"/>
+    </row>
+    <row r="58" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C58" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G39" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F40" s="18" t="s">
+      <c r="D58" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F58" s="25"/>
+    </row>
+    <row r="59" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C59" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G40" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F41" s="18" t="s">
+      <c r="D59" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="F59" s="25"/>
+      <c r="G59" s="20"/>
+    </row>
+    <row r="60" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C60" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G41" s="8" t="s">
+      <c r="D60" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="42" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F42" s="18" t="s">
+      <c r="E60" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="F60" s="25"/>
+      <c r="G60" s="18"/>
+    </row>
+    <row r="61" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C61" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G42" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F43" s="19" t="s">
+      <c r="D61" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="F61" s="25"/>
+    </row>
+    <row r="62" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C62" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="G43" s="9" t="s">
+      <c r="D62" s="9" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="45" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F45" s="2" t="s">
+      <c r="E62" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="F62" s="25"/>
+    </row>
+    <row r="64" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C64" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G45" s="3" t="s">
+      <c r="D64" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F46" s="17" t="s">
+      <c r="E64" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F64" s="26"/>
+    </row>
+    <row r="65" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C65" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G46" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F47" s="25" t="s">
+      <c r="D65" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="F65" s="25"/>
+    </row>
+    <row r="66" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C66" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="G47" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F48" s="19" t="s">
+      <c r="D66" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="F66" s="25"/>
+    </row>
+    <row r="67" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C67" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G48" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F50" s="2" t="s">
+      <c r="D67" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="F67" s="25"/>
+    </row>
+    <row r="69" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C69" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G50" s="3" t="s">
+      <c r="D69" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="51" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F51" s="17" t="s">
+      <c r="E69" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="F69" s="33"/>
+      <c r="G69" s="33"/>
+      <c r="H69" s="33"/>
+    </row>
+    <row r="70" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C70" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G51" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F52" s="25" t="s">
+      <c r="D70" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="F70" s="25"/>
+      <c r="G70" s="25"/>
+      <c r="H70" s="25"/>
+    </row>
+    <row r="71" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C71" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="G52" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F53" s="19" t="s">
+      <c r="D71" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="F71" s="25"/>
+      <c r="G71" s="25"/>
+      <c r="H71" s="25"/>
+    </row>
+    <row r="72" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C72" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G53" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F55" s="21" t="s">
+      <c r="D72" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="F72" s="25"/>
+      <c r="G72" s="25"/>
+      <c r="H72" s="25"/>
+    </row>
+    <row r="74" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C74" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="G55" s="20" t="s">
+      <c r="D74" s="16" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="56" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F56" s="4" t="s">
+      <c r="E74" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="F74" s="33"/>
+      <c r="G74" s="33"/>
+      <c r="H74" s="33"/>
+      <c r="I74" s="33"/>
+      <c r="J74" s="33"/>
+    </row>
+    <row r="75" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C75" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G56" s="7" t="s">
+      <c r="D75" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="57" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F57" s="10" t="s">
+      <c r="E75" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F75" s="25"/>
+      <c r="G75" s="25"/>
+      <c r="H75" s="25"/>
+      <c r="I75" s="25"/>
+      <c r="J75" s="25"/>
+    </row>
+    <row r="76" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C76" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G57" s="8" t="s">
+      <c r="D76" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="58" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F58" s="6" t="s">
+      <c r="E76" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="F76" s="25"/>
+      <c r="G76" s="25"/>
+      <c r="H76" s="25"/>
+      <c r="I76" s="25"/>
+      <c r="J76" s="25"/>
+    </row>
+    <row r="77" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C77" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G58" s="9" t="s">
+      <c r="D77" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="59" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F59" s="22"/>
-      <c r="G59" s="26"/>
-    </row>
-    <row r="60" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F60" s="23"/>
-      <c r="G60" s="23"/>
+      <c r="E77" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="F77" s="25"/>
+      <c r="G77" s="25"/>
+      <c r="H77" s="25"/>
+      <c r="I77" s="25"/>
+      <c r="J77" s="25"/>
     </row>
   </sheetData>
+  <mergeCells count="64">
+    <mergeCell ref="E76:J76"/>
+    <mergeCell ref="E77:J77"/>
+    <mergeCell ref="E69:H69"/>
+    <mergeCell ref="E70:H70"/>
+    <mergeCell ref="E71:H71"/>
+    <mergeCell ref="E72:H72"/>
+    <mergeCell ref="E74:J74"/>
+    <mergeCell ref="E75:J75"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E34:H34"/>
+    <mergeCell ref="E33:H33"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E29:H29"/>
+    <mergeCell ref="E30:H30"/>
+    <mergeCell ref="E31:H31"/>
+    <mergeCell ref="E32:H32"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>